<commit_message>
chore: cleanup project - remove temp files, scripts, and update .gitignore
</commit_message>
<xml_diff>
--- a/testdata/דולינה_גרופ_2025-10-12.xlsx
+++ b/testdata/דולינה_גרופ_2025-10-12.xlsx
@@ -132,7 +132,7 @@
     <t>קמעונאי</t>
   </si>
   <si>
-    <t>J001</t>
+    <t>H527</t>
   </si>
   <si>
     <t>עולי גורדום 2</t>
@@ -219,7 +219,7 @@
     <t>יוסי דוידוב מינימרקט ויקטוריה בע"מ</t>
   </si>
   <si>
-    <t>J301</t>
+    <t>J1207</t>
   </si>
   <si>
     <t>הרצל 101</t>

</xml_diff>